<commit_message>
Add automatic testng listeners
</commit_message>
<xml_diff>
--- a/src/test/resources/setup/Setup.xlsx
+++ b/src/test/resources/setup/Setup.xlsx
@@ -986,7 +986,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1009,7 +1009,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1017,7 +1017,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
Added options to automation setup excel
</commit_message>
<xml_diff>
--- a/src/test/resources/setup/Setup.xlsx
+++ b/src/test/resources/setup/Setup.xlsx
@@ -27,12 +27,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Attribute</t>
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Open allure</t>
   </si>
   <si>
     <t>Headless</t>
@@ -42,6 +51,12 @@
   </si>
   <si>
     <t>Extension</t>
+  </si>
+  <si>
+    <t>No sandbox</t>
+  </si>
+  <si>
+    <t>Disable Dev Shm Usage</t>
   </si>
 </sst>
 </file>
@@ -983,15 +998,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="23.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="10.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="11.7142857142857" customWidth="1"/>
   </cols>
@@ -1008,29 +1023,64 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="b">
+        <v>4</v>
+      </c>
+      <c r="B3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="b">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"Chrome,Firefox,Edge,All"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B4:B8 B14:B1048576">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixed mvn package creation
</commit_message>
<xml_diff>
--- a/src/test/resources/setup/Setup.xlsx
+++ b/src/test/resources/setup/Setup.xlsx
@@ -38,7 +38,7 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>All</t>
+    <t>Chrome</t>
   </si>
   <si>
     <t>Open allure</t>
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -1032,7 +1032,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
Added docker yaml file
</commit_message>
<xml_diff>
--- a/src/test/resources/setup/Setup.xlsx
+++ b/src/test/resources/setup/Setup.xlsx
@@ -38,7 +38,7 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>Chrome</t>
+    <t>All</t>
   </si>
   <si>
     <t>Open allure</t>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1038,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>